<commit_message>
Lige omdøbt module til state. Rasmus opdaterer reset_settings()
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/techdata_new2_simpleEOP.xlsx
+++ b/examples/Abatement/Data/techdata_new2_simpleEOP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="inputdisp" sheetId="1" r:id="rId1"/>
@@ -581,7 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
     </sheetView>
@@ -1078,9 +1078,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,10 +1213,13 @@
         <v>65</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="G3">
         <v>0.25</v>

</xml_diff>